<commit_message>
Update excel sheet and add plots
</commit_message>
<xml_diff>
--- a/hpc_prog1_analysis.xlsx
+++ b/hpc_prog1_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongc\Google Drive\Georgia Tech\spring2019\cx4220\hw2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wongc\Documents\GitHub\HPC_PI_Approx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0088527-18EA-4728-8CED-D6A740422FF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807ACA85-AB29-4010-A661-83AAA8916444}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" firstSheet="1" activeTab="2" xr2:uid="{779A0E9D-636A-45EF-B129-D6E552138C48}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{779A0E9D-636A-45EF-B129-D6E552138C48}"/>
   </bookViews>
   <sheets>
     <sheet name="speedup analysis" sheetId="5" r:id="rId1"/>
@@ -110,9 +110,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,8 +161,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,12 +193,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,22 +219,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -543,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F6896B-12EF-4EE7-9C13-35C83646555F}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,9 +669,9 @@
       <c r="A6" s="3">
         <v>25000000</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6">
         <f>'R=100,P=2'!$E$31</f>
-        <v>#DIV/0!</v>
+        <v>139.49807719999998</v>
       </c>
       <c r="C6">
         <f>'R=100,P=4'!$E$31</f>
@@ -679,9 +690,9 @@
       <c r="A7" s="3">
         <v>30000000</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7">
         <f>'R=100,P=2'!$E$37</f>
-        <v>#DIV/0!</v>
+        <v>166.81146759999999</v>
       </c>
       <c r="C7">
         <f>'R=100,P=4'!$E$37</f>
@@ -700,23 +711,23 @@
       <c r="A8" s="3">
         <v>35000000</v>
       </c>
-      <c r="B8" s="10" t="e">
+      <c r="B8" s="11">
         <f>'R=100,P=2'!$E$43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C8" s="10" t="e">
+        <v>194.48161999999999</v>
+      </c>
+      <c r="C8" s="11">
         <f>'R=100,P=4'!$E$43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="10">
+        <v>97.377161999999998</v>
+      </c>
+      <c r="D8" s="11">
         <f>'R=100,P=8'!$E$43</f>
         <v>49.395214000000003</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <f>'R=100,P=16'!$E$43</f>
         <v>24.252800000000001</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -724,23 +735,23 @@
       <c r="A9" s="3">
         <v>40000000</v>
       </c>
-      <c r="B9" s="10" t="e">
+      <c r="B9" s="11">
         <f>'R=100,P=2'!$E$49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" s="10" t="e">
+        <v>226.73752500000001</v>
+      </c>
+      <c r="C9" s="11">
         <f>'R=100,P=4'!$E$49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="10">
+        <v>110.83343499999999</v>
+      </c>
+      <c r="D9" s="11">
         <f>'R=100,P=8'!$E$49</f>
         <v>56.075479999999999</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="11">
         <f>'R=100,P=16'!$E$49</f>
         <v>28.064344999999999</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -754,9 +765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF756FF-27AD-4DD1-A979-94E09C6FCAA3}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,9 +1372,15 @@
       <c r="D26">
         <v>2</v>
       </c>
+      <c r="E26">
+        <v>140.63112699999999</v>
+      </c>
+      <c r="F26">
+        <v>3.1416149999999998</v>
+      </c>
       <c r="G26">
         <f>ABS((PI()-F26)/PI())</f>
-        <v>1</v>
+        <v>7.1130832895136352E-6</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1379,9 +1396,15 @@
       <c r="D27">
         <v>2</v>
       </c>
+      <c r="E27">
+        <v>139.51623599999999</v>
+      </c>
+      <c r="F27">
+        <v>3.1416759999999999</v>
+      </c>
       <c r="G27">
         <f t="shared" ref="G27:G30" si="4">ABS((PI()-F27)/PI())</f>
-        <v>1</v>
+        <v>2.652998634675312E-5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1397,9 +1420,15 @@
       <c r="D28">
         <v>2</v>
       </c>
+      <c r="E28">
+        <v>139.18846300000001</v>
+      </c>
+      <c r="F28">
+        <v>3.1415489999999999</v>
+      </c>
       <c r="G28">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.3895369198584551E-5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1415,9 +1444,15 @@
       <c r="D29">
         <v>2</v>
       </c>
+      <c r="E29">
+        <v>138.856157</v>
+      </c>
+      <c r="F29">
+        <v>3.1416210000000002</v>
+      </c>
       <c r="G29">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>9.0229426067419782E-6</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1433,9 +1468,15 @@
       <c r="D30">
         <v>2</v>
       </c>
+      <c r="E30">
+        <v>139.29840300000001</v>
+      </c>
+      <c r="F30">
+        <v>3.1416189999999999</v>
+      </c>
       <c r="G30">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>8.3863228342854112E-6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1445,17 +1486,17 @@
       <c r="B31" s="7"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6" t="e">
+      <c r="E31" s="6">
         <f>AVERAGE(E26:E30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="6" t="e">
+        <v>139.49807719999998</v>
+      </c>
+      <c r="F31" s="6">
         <f>AVERAGE(F26:F30)</f>
-        <v>#DIV/0!</v>
+        <v>3.141616</v>
       </c>
       <c r="G31" s="6">
         <f>AVERAGE(G26:G30)</f>
-        <v>1</v>
+        <v>1.2989540855175739E-5</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1471,9 +1512,15 @@
       <c r="D32">
         <v>2</v>
       </c>
+      <c r="E32">
+        <v>167.20078899999999</v>
+      </c>
+      <c r="F32">
+        <v>3.1415980000000001</v>
+      </c>
       <c r="G32">
         <f>ABS((PI()-F32)/PI())</f>
-        <v>1</v>
+        <v>1.7018152244809655E-6</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1489,9 +1536,15 @@
       <c r="D33">
         <v>2</v>
       </c>
+      <c r="E33">
+        <v>166.39612700000001</v>
+      </c>
+      <c r="F33">
+        <v>3.1416369999999998</v>
+      </c>
       <c r="G33">
         <f t="shared" ref="G33:G36" si="5">ABS((PI()-F33)/PI())</f>
-        <v>1</v>
+        <v>1.4115900785546365E-5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1507,9 +1560,15 @@
       <c r="D34">
         <v>2</v>
       </c>
+      <c r="E34">
+        <v>167.19723400000001</v>
+      </c>
+      <c r="F34">
+        <v>3.1416240000000002</v>
+      </c>
       <c r="G34">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>9.977872265285469E-6</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1525,9 +1584,15 @@
       <c r="D35">
         <v>2</v>
       </c>
+      <c r="E35">
+        <v>166.43255300000001</v>
+      </c>
+      <c r="F35">
+        <v>3.1415839999999999</v>
+      </c>
       <c r="G35">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2.75452318214957E-6</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1543,9 +1608,15 @@
       <c r="D36">
         <v>2</v>
       </c>
+      <c r="E36">
+        <v>166.830635</v>
+      </c>
+      <c r="F36">
+        <v>3.1415250000000001</v>
+      </c>
       <c r="G36">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2.1534806466932488E-5</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1555,17 +1626,17 @@
       <c r="B37" s="7"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="6" t="e">
+      <c r="E37" s="6">
         <f>AVERAGE(E32:E36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F37" s="6" t="e">
+        <v>166.81146759999999</v>
+      </c>
+      <c r="F37" s="6">
         <f>AVERAGE(F32:F36)</f>
-        <v>#DIV/0!</v>
+        <v>3.1415935999999998</v>
       </c>
       <c r="G37" s="6">
         <f>AVERAGE(G32:G36)</f>
-        <v>1</v>
+        <v>1.0016983584878972E-5</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1581,9 +1652,15 @@
       <c r="D38">
         <v>2</v>
       </c>
+      <c r="E38">
+        <v>194.48161999999999</v>
+      </c>
+      <c r="F38" s="10">
+        <v>-3.3869280000000002</v>
+      </c>
       <c r="G38">
         <f>ABS((PI()-F38)/PI())</f>
-        <v>1</v>
+        <v>2.0780926661926937</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1598,10 +1675,6 @@
       </c>
       <c r="D39">
         <v>2</v>
-      </c>
-      <c r="G39">
-        <f t="shared" ref="G39:G42" si="6">ABS((PI()-F39)/PI())</f>
-        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1617,10 +1690,6 @@
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -1634,10 +1703,6 @@
       </c>
       <c r="D41">
         <v>2</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1653,10 +1718,6 @@
       <c r="D42">
         <v>2</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
@@ -1665,17 +1726,17 @@
       <c r="B43" s="7"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="6" t="e">
+      <c r="E43" s="6">
         <f>AVERAGE(E38:E42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="6" t="e">
+        <v>194.48161999999999</v>
+      </c>
+      <c r="F43" s="6">
         <f>AVERAGE(F38:F42)</f>
-        <v>#DIV/0!</v>
+        <v>-3.3869280000000002</v>
       </c>
       <c r="G43" s="6">
         <f>AVERAGE(G38:G42)</f>
-        <v>1</v>
+        <v>2.0780926661926937</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1691,9 +1752,15 @@
       <c r="D44">
         <v>2</v>
       </c>
+      <c r="E44">
+        <v>226.73752500000001</v>
+      </c>
+      <c r="F44" s="10">
+        <v>-4.5754010000000003</v>
+      </c>
       <c r="G44">
         <f>ABS((PI()-F44)/PI())</f>
-        <v>1</v>
+        <v>2.4563953715552023</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1708,10 +1775,6 @@
       </c>
       <c r="D45">
         <v>2</v>
-      </c>
-      <c r="G45">
-        <f t="shared" ref="G45:G48" si="7">ABS((PI()-F45)/PI())</f>
-        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1727,10 +1790,6 @@
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
@@ -1744,10 +1803,6 @@
       </c>
       <c r="D47">
         <v>2</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1763,10 +1818,6 @@
       <c r="D48">
         <v>2</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
@@ -1775,17 +1826,17 @@
       <c r="B49" s="7"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="6" t="e">
+      <c r="E49" s="6">
         <f>AVERAGE(E44:E48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F49" s="6" t="e">
+        <v>226.73752500000001</v>
+      </c>
+      <c r="F49" s="6">
         <f>AVERAGE(F44:F48)</f>
-        <v>#DIV/0!</v>
+        <v>-4.5754010000000003</v>
       </c>
       <c r="G49" s="6">
         <f>AVERAGE(G44:G48)</f>
-        <v>1</v>
+        <v>2.4563953715552023</v>
       </c>
     </row>
   </sheetData>
@@ -1798,8 +1849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBD7B61-A568-476E-97BA-813CF7295A71}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2684,9 +2736,15 @@
       <c r="D38">
         <v>4</v>
       </c>
+      <c r="E38">
+        <v>97.377161999999998</v>
+      </c>
+      <c r="F38" s="10">
+        <v>-3.3868939999999998</v>
+      </c>
       <c r="G38">
         <f>ABS((PI()-F38)/PI())</f>
-        <v>1</v>
+        <v>2.0780818436565633</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -2701,10 +2759,6 @@
       </c>
       <c r="D39">
         <v>4</v>
-      </c>
-      <c r="G39">
-        <f t="shared" ref="G39:G42" si="6">ABS((PI()-F39)/PI())</f>
-        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -2720,10 +2774,6 @@
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -2737,10 +2787,6 @@
       </c>
       <c r="D41">
         <v>4</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -2756,10 +2802,6 @@
       <c r="D42">
         <v>4</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
@@ -2768,17 +2810,17 @@
       <c r="B43" s="7"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="6" t="e">
+      <c r="E43" s="6">
         <f>AVERAGE(E38:E42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" s="6" t="e">
+        <v>97.377161999999998</v>
+      </c>
+      <c r="F43" s="6">
         <f>AVERAGE(F38:F42)</f>
-        <v>#DIV/0!</v>
+        <v>-3.3868939999999998</v>
       </c>
       <c r="G43" s="6">
         <f>AVERAGE(G38:G42)</f>
-        <v>1</v>
+        <v>2.0780818436565633</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2794,9 +2836,15 @@
       <c r="D44">
         <v>4</v>
       </c>
+      <c r="E44">
+        <v>110.83343499999999</v>
+      </c>
+      <c r="F44" s="10">
+        <v>-4.5753690000000002</v>
+      </c>
       <c r="G44">
         <f>ABS((PI()-F44)/PI())</f>
-        <v>1</v>
+        <v>2.4563851856388443</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -2811,10 +2859,6 @@
       </c>
       <c r="D45">
         <v>4</v>
-      </c>
-      <c r="G45">
-        <f t="shared" ref="G45:G48" si="7">ABS((PI()-F45)/PI())</f>
-        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2830,10 +2874,6 @@
       <c r="D46">
         <v>4</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
@@ -2847,10 +2887,6 @@
       </c>
       <c r="D47">
         <v>4</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -2866,10 +2902,6 @@
       <c r="D48">
         <v>4</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
@@ -2878,23 +2910,23 @@
       <c r="B49" s="7"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="6" t="e">
+      <c r="E49" s="6">
         <f>AVERAGE(E44:E48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F49" s="6" t="e">
+        <v>110.83343499999999</v>
+      </c>
+      <c r="F49" s="6">
         <f>AVERAGE(F44:F48)</f>
-        <v>#DIV/0!</v>
+        <v>-4.5753690000000002</v>
       </c>
       <c r="G49" s="6">
         <f>AVERAGE(G44:G48)</f>
-        <v>1</v>
+        <v>2.4563851856388443</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G7" formula="1"/>
+    <ignoredError sqref="G7 G31" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2903,8 +2935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9577F33C-990F-4E83-9752-11E7E2536153}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3792,7 +3825,7 @@
       <c r="E38">
         <v>49.395214000000003</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="11">
         <v>-3.3869050000000001</v>
       </c>
       <c r="G38">
@@ -3813,10 +3846,6 @@
       <c r="D39">
         <v>8</v>
       </c>
-      <c r="G39">
-        <f t="shared" ref="G39:G42" si="6">ABS((PI()-F39)/PI())</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
@@ -3831,10 +3860,6 @@
       <c r="D40">
         <v>8</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -3848,10 +3873,6 @@
       </c>
       <c r="D41">
         <v>8</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -3866,10 +3887,6 @@
       </c>
       <c r="D42">
         <v>8</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -3889,7 +3906,7 @@
       </c>
       <c r="G43" s="6">
         <f>AVERAGE(G38:G42)</f>
-        <v>1.2156170690130623</v>
+        <v>2.0780853450653116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -3908,7 +3925,7 @@
       <c r="E44">
         <v>56.075479999999999</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="11">
         <v>-4.5753029999999999</v>
       </c>
       <c r="G44">
@@ -3929,10 +3946,6 @@
       <c r="D45">
         <v>8</v>
       </c>
-      <c r="G45">
-        <f t="shared" ref="G45:G48" si="7">ABS((PI()-F45)/PI())</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
@@ -3947,10 +3960,6 @@
       <c r="D46">
         <v>8</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
@@ -3964,10 +3973,6 @@
       </c>
       <c r="D47">
         <v>8</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -3982,10 +3987,6 @@
       </c>
       <c r="D48">
         <v>8</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -4005,7 +4006,7 @@
       </c>
       <c r="G49" s="6">
         <f>AVERAGE(G44:G48)</f>
-        <v>1.2912728354372711</v>
+        <v>2.456364177186356</v>
       </c>
     </row>
   </sheetData>
@@ -4018,7 +4019,8 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4906,7 +4908,7 @@
       <c r="E38">
         <v>24.252800000000001</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="11">
         <v>-3.386892</v>
       </c>
       <c r="G38">
@@ -4927,10 +4929,6 @@
       <c r="D39">
         <v>16</v>
       </c>
-      <c r="G39">
-        <f t="shared" ref="G39:G42" si="6">ABS((PI()-F39)/PI())</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
@@ -4945,10 +4943,6 @@
       <c r="D40">
         <v>16</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -4962,10 +4956,6 @@
       </c>
       <c r="D41">
         <v>16</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -4980,10 +4970,6 @@
       </c>
       <c r="D42">
         <v>16</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="6"/>
-        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -5003,7 +4989,7 @@
       </c>
       <c r="G43" s="6">
         <f>AVERAGE(G38:G42)</f>
-        <v>1.2156162414073581</v>
+        <v>2.0780812070367909</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -5022,7 +5008,7 @@
       <c r="E44">
         <v>28.064344999999999</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="11">
         <v>-4.5752439999999996</v>
       </c>
       <c r="G44">
@@ -5043,10 +5029,6 @@
       <c r="D45">
         <v>16</v>
       </c>
-      <c r="G45">
-        <f t="shared" ref="G45:G48" si="7">ABS((PI()-F45)/PI())</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
@@ -5061,10 +5043,6 @@
       <c r="D46">
         <v>16</v>
       </c>
-      <c r="G46">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
@@ -5078,10 +5056,6 @@
       </c>
       <c r="D47">
         <v>16</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -5096,10 +5070,6 @@
       </c>
       <c r="D48">
         <v>16</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="7"/>
-        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -5119,7 +5089,7 @@
       </c>
       <c r="G49" s="6">
         <f>AVERAGE(G44:G48)</f>
-        <v>1.2912690793806143</v>
+        <v>2.4563453969030711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>